<commit_message>
Dodanie podziału treningu na części
</commit_message>
<xml_diff>
--- a/Przykladowy Folder/wyniki/wyniki_Kusztal_15.01.2025_1.xlsx
+++ b/Przykladowy Folder/wyniki/wyniki_Kusztal_15.01.2025_1.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,12 +463,15 @@
           <t>Velocity_Bin</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Trening</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>15.01.2025 11:22</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>45672.47361111111</v>
       </c>
       <c r="B2" t="n">
         <v>1109.4</v>
@@ -480,12 +487,15 @@
           <t>10-15</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Duża Gra</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>15.01.2025 11:43</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>45672.48819444444</v>
       </c>
       <c r="B3" t="n">
         <v>2345.7</v>
@@ -501,12 +511,15 @@
           <t>10-15</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Duża Gra</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>15.01.2025 11:51</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>45672.49375</v>
       </c>
       <c r="B4" t="n">
         <v>2841.7</v>
@@ -522,12 +535,15 @@
           <t>10-15</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Duża Gra</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>15.01.2025 11:09</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>45672.46458333333</v>
       </c>
       <c r="B5" t="n">
         <v>340.4</v>
@@ -543,12 +559,15 @@
           <t>5-10</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Duża Gra</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>15.01.2025 11:17</t>
-        </is>
+      <c r="A6" s="2" t="n">
+        <v>45672.47013888889</v>
       </c>
       <c r="B6" t="n">
         <v>795.7</v>
@@ -564,12 +583,15 @@
           <t>5-10</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Duża Gra</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>15.01.2025 11:22</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>45672.47361111111</v>
       </c>
       <c r="B7" t="n">
         <v>1109.2</v>
@@ -583,6 +605,155 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>5-10</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Duża Gra</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45672.46388888889</v>
+      </c>
+      <c r="B8" t="n">
+        <v>279.1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10.87</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9338212012857143</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>10-15</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Mała Gra</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45672.46458333333</v>
+      </c>
+      <c r="B9" t="n">
+        <v>340.6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>11.29</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3.156308037857143</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>10-15</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Mała Gra</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45672.46527777778</v>
+      </c>
+      <c r="B10" t="n">
+        <v>392.2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3.135422025571429</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10-15</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Mała Gra</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45672.46458333333</v>
+      </c>
+      <c r="B11" t="n">
+        <v>340.4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.996093545714285</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>5-10</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Mała Gra</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45672.46527777778</v>
+      </c>
+      <c r="B12" t="n">
+        <v>388.1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.776477507142857</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5-10</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Mała Gra</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45672.46527777778</v>
+      </c>
+      <c r="B13" t="n">
+        <v>391.9</v>
+      </c>
+      <c r="C13" t="n">
+        <v>8.73</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.766690067142857</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>5-10</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Mała Gra</t>
         </is>
       </c>
     </row>

</xml_diff>